<commit_message>
Update to framawork 7.0M2 and and bcaktasting formule
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_RISK_EW/03_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_RISK_EW/03_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Action</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>updateOutputIrisTable</t>
+  </si>
+  <si>
+    <t>backTesting</t>
   </si>
 </sst>
 </file>
@@ -715,7 +718,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -755,10 +758,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -826,6 +829,23 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -838,7 +858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -868,12 +890,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -991,15 +1010,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1021,16 +1050,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>